<commit_message>
Random forest and ensembling
</commit_message>
<xml_diff>
--- a/freeCodeCamp/SalesCompetition/ModelTracking.xlsx
+++ b/freeCodeCamp/SalesCompetition/ModelTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\ML\freeCodeCamp\SalesCompetition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1C0831-0E66-4E75-BE26-5F807B81AA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BBFDBD-6730-457B-9D2B-B0ED3AEE870B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">HyperParameters </t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Training Score</t>
   </si>
   <si>
@@ -88,6 +85,28 @@
   </si>
   <si>
     <t>Tree based model generally overfit themselves, Still validation loss is much less than Linear Models</t>
+  </si>
+  <si>
+    <t>Random Forest Regessor</t>
+  </si>
+  <si>
+    <t>Random state = 61
+n_jobs = -1</t>
+  </si>
+  <si>
+    <t>This Prouces the best result as of now and can be tuned for better accuracy</t>
+  </si>
+  <si>
+    <t>80 - Random Forest
+20 - Ridge</t>
+  </si>
+  <si>
+    <t>n_jobs=-1, random_state=len(x_train), n_estimators=20
+-----
+None</t>
+  </si>
+  <si>
+    <t>The combination is better than many of the models but not more than that of the Random forest's Original Output</t>
   </si>
 </sst>
 </file>
@@ -137,15 +156,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,75 +450,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="5" width="17" style="3"/>
     <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="45.77734375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
-        <v>46447</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" s="4">
+        <v>46447</v>
       </c>
       <c r="D2" s="3">
         <v>2740.0200553867098</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>2811.5238054135302</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6">
-        <v>46447</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>46447</v>
       </c>
       <c r="D3" s="3">
         <v>2740.1672811348399</v>
@@ -503,18 +523,15 @@
         <v>2811.5202521932301</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="6">
-        <v>46447</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="4">
+        <v>46447</v>
       </c>
       <c r="D4" s="3">
         <v>2740.0168943417598</v>
@@ -523,18 +540,15 @@
         <v>2740.0168943417598</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6">
-        <v>46447</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="4">
+        <v>46447</v>
       </c>
       <c r="D5" s="3">
         <v>2878.8229248586999</v>
@@ -543,18 +557,15 @@
         <v>2974.30546</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="6">
-        <v>46447</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>46447</v>
       </c>
       <c r="D6" s="3">
         <v>2740.2711653384099</v>
@@ -563,18 +574,18 @@
         <v>2812.0258406384401</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4">
+        <v>46447</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="6">
-        <v>46447</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -582,11 +593,52 @@
       <c r="E7" s="3">
         <v>1553.76681804072</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>17</v>
+      </c>
+      <c r="B8" s="4">
+        <v>46447</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>474.37886939340001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1367.15354958689</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="8">
+        <v>46447</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3">
+        <v>812.04496192446902</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1431.3805071645099</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>